<commit_message>
Update types in the M1 test plan. Removed .pdf version.
</commit_message>
<xml_diff>
--- a/tests/M01_demonstration_test_plan_course.xlsx
+++ b/tests/M01_demonstration_test_plan_course.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daltenburg\repos\comp-2327-demonstation\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daltenburg\repos\WI2025\isd\fte03\demonstration\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62869874-4EF6-4BF1-BE99-43705A362184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A32E6-D90B-4FA1-9202-F67F5E67F69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$14</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -183,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -242,7 +245,42 @@
     <t>Course</t>
   </si>
   <si>
-    <t>Exception raised when credit_hours is not an int.</t>
+    <t>Damien Altenburg</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>name = "intermediate software development"
+department = Department.COMPUTER_SCIENCE
+credit_hours = 90</t>
+  </si>
+  <si>
+    <t>Object initialized with the correct state</t>
+  </si>
+  <si>
+    <t>name = ""
+department = Department.COMPUTER_SCIENCE
+credit_hours = 90</t>
+  </si>
+  <si>
+    <t>name = "intermediate software development"
+department = "computer science"
+credit_hours = 90</t>
+  </si>
+  <si>
+    <t>Exception raised when credit hours is not an int.</t>
+  </si>
+  <si>
+    <t>name = "intermediate software development"
+department = Department.COMPUTER_SCIENCE
+credit_hours = 34.5</t>
+  </si>
+  <si>
+    <t>Object initialized.
+name = "intermediate software development"
+department = Department.COMPUTER_SCIENCE
+credit_hours = 90</t>
   </si>
   <si>
     <t>Returns name attribute</t>
@@ -255,6 +293,26 @@
   </si>
   <si>
     <t>Returns string in expected format.</t>
+  </si>
+  <si>
+    <t>"intermediate software development"</t>
+  </si>
+  <si>
+    <t>Department.COMPUTER_SCIENCE</t>
+  </si>
+  <si>
+    <t>ValueError: Name cannot be blank.</t>
+  </si>
+  <si>
+    <t>ValueError: Department is not valid.</t>
+  </si>
+  <si>
+    <t>"Course: Intermediate Software Development
+Department: Computer Science
+Credit Hours: 90"</t>
+  </si>
+  <si>
+    <t>ValueError: Credit Hours must be numeric.</t>
   </si>
 </sst>
 </file>
@@ -565,11 +623,10 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -579,52 +636,78 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1088,6 +1171,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0"/>
@@ -1097,9 +1183,9 @@
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1119,7 +1205,9 @@
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1165,11 +1253,17 @@
       <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1180,9 +1274,15 @@
       <c r="D8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -1195,9 +1295,15 @@
       <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -1208,13 +1314,19 @@
         <v>8</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
         <v>5</v>
       </c>
@@ -1222,13 +1334,19 @@
         <v>15</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>6</v>
       </c>
@@ -1236,13 +1354,19 @@
         <v>16</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1250,13 +1374,19 @@
         <v>17</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B14" s="12">
         <v>8</v>
       </c>
@@ -1264,131 +1394,137 @@
         <v>12</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
         <v>9</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <v>10</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12">
         <v>11</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12">
         <v>12</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
         <v>13</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="12">
         <v>14</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="12">
         <v>15</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <v>16</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>17</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>18</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
         <v>19</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="12">
         <v>20</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="19" t="s">
@@ -1408,9 +1544,10 @@
     <mergeCell ref="B28:G28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup scale="57" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>